<commit_message>
Preenchimento e correção do documento STE_PA_Planilha de Avaliação -Sprint-02 (Nível F MPS.br)
</commit_message>
<xml_diff>
--- a/docs/Project Docs/STE_PA_Planilha de Avaliação -Sprint-02 (Nível F MPS.br).xlsx
+++ b/docs/Project Docs/STE_PA_Planilha de Avaliação -Sprint-02 (Nível F MPS.br).xlsx
@@ -22,8 +22,148 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Bruno dos Santos Messias</author>
+  </authors>
+  <commentList>
+    <comment ref="C18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bruno dos Santos Messias:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Atende parcialmente pois não foram defindos uma análise para avaliação ou aceitação dos requisitos</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Bruno dos Santos Messias</author>
+  </authors>
+  <commentList>
+    <comment ref="C39" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bruno dos Santos Messias:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Atede parcialmente pos não são definidos marcos ou ponto de controle no cronograma</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C46" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bruno dos Santos Messias:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Atende parcialmente pois não é feita uma análise para determinar a probabilidade, o impacto, o grau de importância e a prioridade de cada risco</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C53" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bruno dos Santos Messias:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Não atende pois não são definidos os requisitos de cada papel e as comepetencias de cada participante</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C130" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bruno dos Santos Messias:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Atende parcialmente pois não comprova que foram tratados com os interessados</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="54">
   <si>
     <t>Gerência de Requisitos</t>
   </si>
@@ -53,7 +193,16 @@
 (iii) que os requisitos foram aceitos pelo cliente ou um representante?</t>
   </si>
   <si>
+    <t>MSL_HU_HistoriasDeUsuario.docx</t>
+  </si>
+  <si>
+    <t>MSL_PP_PlanoDoProjeto.docx - Seção 10</t>
+  </si>
+  <si>
     <t>(A,AP,NA)</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
   <si>
     <t>GRE 2. Os requisitos são avaliados com base em critérios objetivos e um comprometimento da equipe técnica com estes requisitos é obtido.
@@ -63,8 +212,20 @@
 (iii) que um novo comprometimento da equipe técnica com os requisitos foi obtido e registrado quando houve mudanças nos requisitos?</t>
   </si>
   <si>
+    <t>Termo de Compromisso - Sprint 2</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
     <t>GRE 3. A rastreabilidade bidirecional entre os requisitos e os produtos de trabalho é estabelecida e mantida.                                
 As evidências apresentadas para este resultado permitem assegurar que foi criada e mantida, ao longo do projeto, a rastreabilidade bidirecional entre os requisitos e demais produtos de trabalho, incluindo os planos do projeto e as unidades de código?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadro do Trello - HU são transformadas em TASK's </t>
+  </si>
+  <si>
+    <t>Registro de Commits - Os commits se iniciam com TASK desenvolvida</t>
   </si>
   <si>
     <t>GRE 4. Revisões em planos e produtos de trabalho do projeto são realizadas visando identificar e corrigir inconsistências em relação aos requisitos.                            
@@ -73,11 +234,17 @@
 (ii) que foram executadas ações para corrigir inconsistências identificadas ao longo do projeto?</t>
   </si>
   <si>
+    <t>Sprint Retrospective</t>
+  </si>
+  <si>
     <t>GRE 5. Mudanças nos requisitos são gerenciadas ao longo do projeto.
 As evidências apresentadas para este resultado permitem assegurar: 
 (i) que existe um histórico das solicitações de mudança em requisitos do projeto, disponível para a equipe do projeto? 
 (ii) que foi realizada uma análise do impacto destas mudanças antes de sua implementação? 
 (iii) que a mudança foi incorporada ao planejamento do projeto antes de ser executada?</t>
+  </si>
+  <si>
+    <t>Quadro do Trello - Lista Request Change on Backlog</t>
   </si>
   <si>
     <t>Gerência de Projetos</t>
@@ -90,12 +257,21 @@
 As evidências apresentadas para este resultado permitem assegurar que o escopo do projeto foi definido?</t>
   </si>
   <si>
+    <t>MSL_PP_PlanoDoProjeto.docx - Seção 1.2</t>
+  </si>
+  <si>
     <t>GPR 2. As tarefas e os produtos de trabalho do projeto são dimensionados utilizando métodos apropriados.
 As evidências apresentadas para este resultado permitem assegurar que o tamanho e/ou a complexidade das tarefas e dos artefatos gerados no projeto foram estimados utilizando métodos adequados (ex: baseados na EAP ou estrutura equivalente, em técnicas de estimativa ou em dados históricos)?</t>
   </si>
   <si>
+    <t>MSL_AR_AtasDeReunião.docx - Sprint Planning</t>
+  </si>
+  <si>
     <t>GPR 3. O modelo e as fases do ciclo de vida do projeto são definidos.
 As evidências apresentadas para este resultado permitem assegurar que  o modelo do ciclo de vida do projeto foi definido, indicando suas fases, as relações de sequência e interdependência entre elas?</t>
+  </si>
+  <si>
+    <t>MSL_PP_PlanoDoProjeto.docx - Seção 6.2</t>
   </si>
   <si>
     <t>GPR 4. (Até o nível F) O esforço e o custo para a execução das tarefas e dos produtos de trabalho são estimados com base em dados históricos ou referências técnicas.
@@ -109,10 +285,19 @@
 (iii) o cronograma estabelece as dependências entre tarefas?</t>
   </si>
   <si>
+    <t>Atualização do Cronograma</t>
+  </si>
+  <si>
+    <t>MSL_CP_CronogramaDoProjeto.xlsx</t>
+  </si>
+  <si>
     <t>GPR 6. Os riscos do projeto são identificados e o seu impacto, probabilidade de ocorrência e prioridade de tratamento são determinados e documentados.
 As evidências apresentadas para este resultado permitem assegurar que: 
 (i) existe uma lista dos riscos identificados para o projeto? 
 (ii) foi realizada uma análise para determinar a probabilidade, o impacto, o grau de importância (exposição) e a prioridade de cada risco?</t>
+  </si>
+  <si>
+    <t>MSL_PP_PlanoDoProjeto.docx - Seção 3</t>
   </si>
   <si>
     <t>GPR 7. Os recursos humanos para o projeto são planejados considerando o perfil e o conhecimento necessários para executá-lo.
@@ -121,16 +306,28 @@
 (ii) foi planejado treinamento, quando necessário?</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>GPR 8. (Até o Nível F) Os recursos e o ambiente de trabalho necessários para executar o projeto são planejados.
 As evidências apresentadas para este resultado permitem assegurar que foram planejados os recursos e o ambiente de trabalho necessários? (obs: aqui trata-se de outros recursos que não recursos humanos).</t>
+  </si>
+  <si>
+    <t>MSL_PP_PlanoDoProjeto.docx - Seção 2</t>
   </si>
   <si>
     <t>GPR 9. Os dados relevantes do projeto são identificados e planejados quanto à forma de coleta, armazenamento e distribuição. Um mecanismo é estabelecido para acessá-los, incluindo, se pertinente, questões de privacidade e segurança.
 As evidências apresentadas para este resultado permitem assegurar que  existe um plano para gerência de dados, que relacione todos os documentos gerados no projeto, sua distribuição, mídia para armazenamento, forma de proteção (segurança e sigilo) e recuperação dos dados?</t>
   </si>
   <si>
+    <t>MSL_PGC_PlanoDeGerênciaDeConfiguração.docx</t>
+  </si>
+  <si>
     <t>GPR 10. Um plano geral para a execução do projeto é estabelecido com a integração de planos específicos.
 As evidências apresentadas para este resultado permitem assegurar que as informações de planejamento do projeto foram documentadas, organizadas e relacionadas entre si, de forma a comporem o plano de projeto?</t>
+  </si>
+  <si>
+    <t>MSL_PP_PlanoDoProjeto.docx</t>
   </si>
   <si>
     <t>GPR 11. A viabilidade de atingir as metas do projeto é explicitamente avaliada  considerando restrições e recursos disponíveis. Se necessário, ajustes são realizados.
@@ -153,6 +350,9 @@
   <si>
     <t>GPR 15. Os riscos são monitorados em relação ao planejado.
 As evidências apresentadas para este resultado permitem assegurar que o projeto foi monitorado ao longo de seu ciclo de vida, comparando o planejado e o realizado em relação aos riscos?</t>
+  </si>
+  <si>
+    <t>MSL_PP_PlanoDoProjeto.docx - Seção 3.2</t>
   </si>
   <si>
     <t>GPR 16. O envolvimento das partes interessadas no projeto é planejado, monitorado e mantido.
@@ -178,7 +378,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -256,6 +456,25 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -743,11 +962,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -808,6 +1028,18 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -863,6 +1095,24 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -904,30 +1154,1184 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+  <cellStyles count="3">
+    <cellStyle name="Célula de Verificação" xfId="1" builtinId="23"/>
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="224">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1066,6 +2470,37 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1782,6 +3217,221 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -2233,11 +3883,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2249,12 +3899,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="27.75" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2278,12 +3928,12 @@
       <c r="Y1" s="2"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2342,12 +3992,12 @@
       <c r="Y3" s="2"/>
     </row>
     <row r="4" spans="1:25" ht="25.5" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2371,12 +4021,12 @@
       <c r="Y4" s="2"/>
     </row>
     <row r="5" spans="1:25" ht="59.25" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2400,9 +4050,14 @@
       <c r="Y5" s="2"/>
     </row>
     <row r="6" spans="1:25" ht="12" customHeight="1">
-      <c r="A6" s="20"/>
+      <c r="A6" s="20" t="s">
+        <v>8</v>
+      </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="11"/>
+      <c r="C6" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_HU_HistoriasDeUsuario.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D6" s="10"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
@@ -2427,9 +4082,14 @@
       <c r="Y6" s="2"/>
     </row>
     <row r="7" spans="1:25" ht="12" customHeight="1">
-      <c r="A7" s="17"/>
+      <c r="A7" s="17" t="s">
+        <v>9</v>
+      </c>
       <c r="B7" s="21"/>
-      <c r="C7" s="10"/>
+      <c r="C7" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_PP_PlanoDoProjeto.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D7" s="10"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
@@ -2534,13 +4194,15 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="11" spans="1:25" ht="17.25" customHeight="1">
       <c r="A11" s="16"/>
       <c r="B11" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="C11" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="26"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2564,12 +4226,12 @@
       <c r="Y11" s="2"/>
     </row>
     <row r="12" spans="1:25" ht="72.75" customHeight="1" thickTop="1">
-      <c r="A12" s="27" t="s">
-        <v>9</v>
+      <c r="A12" s="31" t="s">
+        <v>12</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2593,9 +4255,14 @@
       <c r="Y12" s="2"/>
     </row>
     <row r="13" spans="1:25" ht="12" customHeight="1">
-      <c r="A13" s="20"/>
+      <c r="A13" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="B13" s="21"/>
-      <c r="C13" s="11"/>
+      <c r="C13" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/Termo%20de%20Compromisso%20-%20Sprint%202", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
@@ -2727,13 +4394,15 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="18" spans="1:25" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A18" s="16"/>
       <c r="B18" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="C18" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="26"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -2757,12 +4426,12 @@
       <c r="Y18" s="2"/>
     </row>
     <row r="19" spans="1:25" ht="43.5" customHeight="1" thickTop="1">
-      <c r="A19" s="24" t="s">
-        <v>10</v>
+      <c r="A19" s="28" t="s">
+        <v>15</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2786,9 +4455,14 @@
       <c r="Y19" s="2"/>
     </row>
     <row r="20" spans="1:25" ht="12" customHeight="1">
-      <c r="A20" s="20"/>
+      <c r="A20" s="25" t="s">
+        <v>16</v>
+      </c>
       <c r="B20" s="21"/>
-      <c r="C20" s="11"/>
+      <c r="C20" s="24" t="str">
+        <f>HYPERLINK("https://trello.com/b/Bc4qaimg/sprint-task-s", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2"/>
@@ -2813,9 +4487,14 @@
       <c r="Y20" s="2"/>
     </row>
     <row r="21" spans="1:25" ht="12" customHeight="1">
-      <c r="A21" s="17"/>
+      <c r="A21" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="B21" s="21"/>
-      <c r="C21" s="10"/>
+      <c r="C21" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/commits/develop2", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D21" s="10"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
@@ -2920,13 +4599,15 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="16"/>
       <c r="B25" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="C25" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="26"/>
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2949,13 +4630,13 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" ht="61.5" customHeight="1" thickTop="1">
-      <c r="A26" s="27" t="s">
-        <v>11</v>
+    <row r="26" spans="1:25" ht="61.5" customHeight="1">
+      <c r="A26" s="31" t="s">
+        <v>18</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="1"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2979,9 +4660,14 @@
       <c r="Y26" s="2"/>
     </row>
     <row r="27" spans="1:25" ht="12" customHeight="1">
-      <c r="A27" s="20"/>
+      <c r="A27" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="B27" s="21"/>
-      <c r="C27" s="11"/>
+      <c r="C27" s="24" t="str">
+        <f>HYPERLINK("https://www.dropbox.com/s/ast9g7enrjgb4jq/Sprint Retrospective - 2ª Iteração.docx?dl=0​", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D27" s="10"/>
       <c r="E27" s="1"/>
       <c r="F27" s="2"/>
@@ -3113,13 +4799,15 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="32" spans="1:25" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A32" s="16"/>
       <c r="B32" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
+      <c r="C32" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="26"/>
       <c r="E32" s="1"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -3142,9 +4830,9 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:25" ht="78.75" customHeight="1" thickTop="1">
+    <row r="33" spans="1:25" ht="60.75" customHeight="1" thickTop="1">
       <c r="A33" s="6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -3172,9 +4860,14 @@
       <c r="Y33" s="2"/>
     </row>
     <row r="34" spans="1:25" ht="12" customHeight="1">
-      <c r="A34" s="20"/>
+      <c r="A34" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="B34" s="21"/>
-      <c r="C34" s="11"/>
+      <c r="C34" s="24" t="str">
+        <f>HYPERLINK("https://trello.com/b/a6Csua2H/backlog​", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D34" s="10"/>
       <c r="E34" s="1"/>
       <c r="F34" s="2"/>
@@ -3309,10 +5002,12 @@
     <row r="39" spans="1:25" ht="12" customHeight="1" thickTop="1" thickBot="1">
       <c r="A39" s="16"/>
       <c r="B39" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
+      <c r="C39" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="26"/>
       <c r="E39" s="1"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -28992,93 +30687,184 @@
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A12:D12"/>
   </mergeCells>
-  <conditionalFormatting sqref="A34:D38">
-    <cfRule type="containsBlanks" dxfId="92" priority="17">
+  <conditionalFormatting sqref="A35:D38 A34:B34 D34">
+    <cfRule type="containsBlanks" dxfId="223" priority="37">
       <formula>LEN(TRIM(A34))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D17">
-    <cfRule type="containsBlanks" dxfId="91" priority="16">
+  <conditionalFormatting sqref="A14:D17 A13:B13 D13">
+    <cfRule type="containsBlanks" dxfId="222" priority="36">
       <formula>LEN(TRIM(A13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="containsText" dxfId="90" priority="14" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="221" priority="34" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="15" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="220" priority="35" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="88" priority="13" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="219" priority="33" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:D10">
-    <cfRule type="containsBlanks" dxfId="87" priority="12">
+    <cfRule type="containsBlanks" dxfId="218" priority="32">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B10">
-    <cfRule type="containsText" dxfId="86" priority="10" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="217" priority="30" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="216" priority="31" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="84" priority="9" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="215" priority="29" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:D24">
-    <cfRule type="containsBlanks" dxfId="83" priority="8">
+  <conditionalFormatting sqref="A22:D24 D20:D21 A20:B21">
+    <cfRule type="containsBlanks" dxfId="214" priority="28">
       <formula>LEN(TRIM(A20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B24">
-    <cfRule type="containsText" dxfId="82" priority="6" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="213" priority="26" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="7" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="212" priority="27" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="80" priority="5" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="211" priority="25" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27:D31">
-    <cfRule type="containsBlanks" dxfId="79" priority="4">
+  <conditionalFormatting sqref="A28:D31 A27:B27 D27">
+    <cfRule type="containsBlanks" dxfId="210" priority="24">
       <formula>LEN(TRIM(A27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:B31">
-    <cfRule type="containsText" dxfId="78" priority="2" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="209" priority="22" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="3" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="208" priority="23" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="76" priority="1" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="207" priority="21" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="containsBlanks" dxfId="206" priority="20">
+      <formula>LEN(TRIM(C13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsBlanks" dxfId="205" priority="19">
+      <formula>LEN(TRIM(C20))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="containsBlanks" dxfId="204" priority="18">
+      <formula>LEN(TRIM(C21))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="containsBlanks" dxfId="203" priority="17">
+      <formula>LEN(TRIM(C27))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsBlanks" dxfId="202" priority="16">
+      <formula>LEN(TRIM(C34))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="containsText" dxfId="201" priority="14" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="200" priority="15" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:D11">
+    <cfRule type="containsText" dxfId="199" priority="13" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="containsText" dxfId="198" priority="11" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="197" priority="12" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:D18">
+    <cfRule type="containsText" dxfId="196" priority="10" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="containsText" dxfId="195" priority="8" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="194" priority="9" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:D25">
+    <cfRule type="containsText" dxfId="193" priority="7" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="containsText" dxfId="192" priority="5" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="191" priority="6" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:D32">
+    <cfRule type="containsText" dxfId="190" priority="4" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="containsText" dxfId="189" priority="2" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="188" priority="3" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:D39">
+    <cfRule type="containsText" dxfId="187" priority="1" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -29090,12 +30876,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A1" s="45" t="s">
-        <v>13</v>
+      <c r="A1" s="55" t="s">
+        <v>22</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -29116,12 +30902,12 @@
       <c r="V1" s="2"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -29172,12 +30958,12 @@
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:22" ht="65.25" customHeight="1">
-      <c r="A4" s="50" t="s">
-        <v>14</v>
+      <c r="A4" s="60" t="s">
+        <v>23</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -29196,12 +30982,12 @@
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="1:22" ht="24" customHeight="1">
-      <c r="A5" s="53" t="s">
-        <v>15</v>
+      <c r="A5" s="63" t="s">
+        <v>24</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -29220,9 +31006,14 @@
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="1:22" ht="12" customHeight="1">
-      <c r="A6" s="20"/>
+      <c r="A6" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="11"/>
+      <c r="C6" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_PP_PlanoDoProjeto.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D6" s="10"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -29329,13 +31120,15 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="11" spans="1:22" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="16"/>
       <c r="B11" s="18" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="C11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="26"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -29354,12 +31147,12 @@
       <c r="T11" s="2"/>
     </row>
     <row r="12" spans="1:22" ht="39" customHeight="1" thickTop="1">
-      <c r="A12" s="42" t="s">
-        <v>16</v>
+      <c r="A12" s="52" t="s">
+        <v>26</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="54"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -29378,9 +31171,14 @@
       <c r="T12" s="2"/>
     </row>
     <row r="13" spans="1:22" ht="12" customHeight="1">
-      <c r="A13" s="20"/>
+      <c r="A13" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="B13" s="21"/>
-      <c r="C13" s="11"/>
+      <c r="C13" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_AR_AtasDeReuni%C3%A3o.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -29487,13 +31285,15 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="18" spans="1:20" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A18" s="16"/>
       <c r="B18" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="C18" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="26"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -29512,12 +31312,12 @@
       <c r="T18" s="2"/>
     </row>
     <row r="19" spans="1:20" ht="39" customHeight="1" thickTop="1">
-      <c r="A19" s="42" t="s">
-        <v>17</v>
+      <c r="A19" s="52" t="s">
+        <v>28</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -29536,9 +31336,14 @@
       <c r="T19" s="2"/>
     </row>
     <row r="20" spans="1:20" ht="12" customHeight="1">
-      <c r="A20" s="20"/>
+      <c r="A20" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="B20" s="21"/>
-      <c r="C20" s="11"/>
+      <c r="C20" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_PP_PlanoDoProjeto.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -29645,13 +31450,15 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="25" spans="1:20" ht="18" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="16"/>
       <c r="B25" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="C25" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="26"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -29670,12 +31477,12 @@
       <c r="T25" s="2"/>
     </row>
     <row r="26" spans="1:20" ht="41.25" customHeight="1" thickTop="1">
-      <c r="A26" s="42" t="s">
-        <v>18</v>
+      <c r="A26" s="52" t="s">
+        <v>30</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="44"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -29694,9 +31501,14 @@
       <c r="T26" s="2"/>
     </row>
     <row r="27" spans="1:20" ht="12" customHeight="1">
-      <c r="A27" s="20"/>
+      <c r="A27" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="B27" s="21"/>
-      <c r="C27" s="11"/>
+      <c r="C27" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_AR_AtasDeReuni%C3%A3o.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D27" s="10"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -29803,13 +31615,15 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
-    <row r="32" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="32" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A32" s="16"/>
       <c r="B32" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
+      <c r="C32" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="26"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -29828,12 +31642,12 @@
       <c r="T32" s="2"/>
     </row>
     <row r="33" spans="1:20" ht="65.25" customHeight="1" thickTop="1">
-      <c r="A33" s="42" t="s">
-        <v>19</v>
+      <c r="A33" s="52" t="s">
+        <v>31</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="44"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="54"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -29852,9 +31666,14 @@
       <c r="T33" s="2"/>
     </row>
     <row r="34" spans="1:20" ht="12" customHeight="1">
-      <c r="A34" s="20"/>
+      <c r="A34" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="B34" s="21"/>
-      <c r="C34" s="11"/>
+      <c r="C34" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/commits/master/docs/Project%20Docs/MSL_CP_CronogramaDoProjeto.xlsx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D34" s="10"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -29874,9 +31693,14 @@
       <c r="T34" s="2"/>
     </row>
     <row r="35" spans="1:20" ht="12" customHeight="1">
-      <c r="A35" s="17"/>
+      <c r="A35" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="B35" s="21"/>
-      <c r="C35" s="10"/>
+      <c r="C35" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/576404957d455644b03d1f04c1d601c97fe000b9/docs/Project%20Docs/MSL_CP_CronogramaDoProjeto.xlsx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D35" s="10"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -29961,13 +31785,15 @@
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
     </row>
-    <row r="39" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="39" spans="1:20" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A39" s="16"/>
       <c r="B39" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
+      <c r="C39" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="26"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -29986,12 +31812,12 @@
       <c r="T39" s="2"/>
     </row>
     <row r="40" spans="1:20" ht="52.5" customHeight="1" thickTop="1">
-      <c r="A40" s="42" t="s">
-        <v>20</v>
+      <c r="A40" s="52" t="s">
+        <v>34</v>
       </c>
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="44"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="54"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -30010,9 +31836,14 @@
       <c r="T40" s="2"/>
     </row>
     <row r="41" spans="1:20" ht="12" customHeight="1">
-      <c r="A41" s="20"/>
+      <c r="A41" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="B41" s="21"/>
-      <c r="C41" s="11"/>
+      <c r="C41" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_PP_PlanoDoProjeto.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D41" s="10"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -30119,13 +31950,15 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
     </row>
-    <row r="46" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="46" spans="1:20" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A46" s="16"/>
       <c r="B46" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
+      <c r="C46" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="26"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -30144,12 +31977,12 @@
       <c r="T46" s="2"/>
     </row>
     <row r="47" spans="1:20" ht="52.5" customHeight="1" thickTop="1">
-      <c r="A47" s="42" t="s">
-        <v>21</v>
+      <c r="A47" s="52" t="s">
+        <v>36</v>
       </c>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="44"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="54"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -30168,9 +32001,14 @@
       <c r="T47" s="2"/>
     </row>
     <row r="48" spans="1:20" ht="12" customHeight="1">
-      <c r="A48" s="20"/>
+      <c r="A48" s="20" t="s">
+        <v>9</v>
+      </c>
       <c r="B48" s="21"/>
-      <c r="C48" s="11"/>
+      <c r="C48" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_PP_PlanoDoProjeto.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D48" s="10"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -30277,13 +32115,15 @@
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
     </row>
-    <row r="53" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="53" spans="1:20" ht="18" customHeight="1" thickTop="1" thickBot="1">
       <c r="A53" s="16"/>
       <c r="B53" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
+      <c r="C53" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" s="26"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -30302,12 +32142,12 @@
       <c r="T53" s="2"/>
     </row>
     <row r="54" spans="1:20" ht="42.75" customHeight="1" thickTop="1">
-      <c r="A54" s="42" t="s">
-        <v>22</v>
+      <c r="A54" s="52" t="s">
+        <v>38</v>
       </c>
-      <c r="B54" s="43"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="44"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="54"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -30326,9 +32166,14 @@
       <c r="T54" s="2"/>
     </row>
     <row r="55" spans="1:20" ht="12" customHeight="1">
-      <c r="A55" s="20"/>
+      <c r="A55" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="B55" s="21"/>
-      <c r="C55" s="11"/>
+      <c r="C55" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_PP_PlanoDoProjeto.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D55" s="10"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
@@ -30435,13 +32280,15 @@
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
     </row>
-    <row r="60" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="60" spans="1:20" ht="18" customHeight="1" thickTop="1" thickBot="1">
       <c r="A60" s="16"/>
       <c r="B60" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+      <c r="C60" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="26"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -30460,12 +32307,12 @@
       <c r="T60" s="2"/>
     </row>
     <row r="61" spans="1:20" ht="53.25" customHeight="1" thickTop="1">
-      <c r="A61" s="42" t="s">
-        <v>23</v>
+      <c r="A61" s="52" t="s">
+        <v>40</v>
       </c>
-      <c r="B61" s="43"/>
-      <c r="C61" s="43"/>
-      <c r="D61" s="44"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="54"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -30484,9 +32331,14 @@
       <c r="T61" s="2"/>
     </row>
     <row r="62" spans="1:20" ht="12" customHeight="1">
-      <c r="A62" s="20"/>
+      <c r="A62" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="B62" s="21"/>
-      <c r="C62" s="11"/>
+      <c r="C62" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/576404957d455644b03d1f04c1d601c97fe000b9/docs/Project%20Docs/MSL_PGC_PlanoDeGer%C3%AAnciaDeConfigura%C3%A7%C3%A3o.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D62" s="10"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -30593,13 +32445,15 @@
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
     </row>
-    <row r="67" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="67" spans="1:20" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A67" s="16"/>
       <c r="B67" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
+      <c r="C67" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="26"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -30618,12 +32472,12 @@
       <c r="T67" s="2"/>
     </row>
     <row r="68" spans="1:20" ht="41.25" customHeight="1" thickTop="1">
-      <c r="A68" s="42" t="s">
-        <v>24</v>
+      <c r="A68" s="52" t="s">
+        <v>42</v>
       </c>
-      <c r="B68" s="43"/>
-      <c r="C68" s="43"/>
-      <c r="D68" s="44"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="53"/>
+      <c r="D68" s="54"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -30642,9 +32496,14 @@
       <c r="T68" s="2"/>
     </row>
     <row r="69" spans="1:20" ht="12" customHeight="1">
-      <c r="A69" s="20"/>
+      <c r="A69" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="B69" s="21"/>
-      <c r="C69" s="11"/>
+      <c r="C69" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_PP_PlanoDoProjeto.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D69" s="10"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -30751,13 +32610,15 @@
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
     </row>
-    <row r="74" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="74" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A74" s="16"/>
       <c r="B74" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
+      <c r="C74" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="26"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -30776,12 +32637,12 @@
       <c r="T74" s="2"/>
     </row>
     <row r="75" spans="1:20" ht="41.25" customHeight="1" thickTop="1">
-      <c r="A75" s="42" t="s">
-        <v>25</v>
+      <c r="A75" s="52" t="s">
+        <v>44</v>
       </c>
-      <c r="B75" s="43"/>
-      <c r="C75" s="43"/>
-      <c r="D75" s="44"/>
+      <c r="B75" s="53"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="54"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -30909,13 +32770,15 @@
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
     </row>
-    <row r="81" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="81" spans="1:20" ht="18" customHeight="1" thickTop="1" thickBot="1">
       <c r="A81" s="16"/>
       <c r="B81" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
+      <c r="C81" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D81" s="26"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -30934,12 +32797,12 @@
       <c r="T81" s="2"/>
     </row>
     <row r="82" spans="1:20" ht="51" customHeight="1" thickTop="1">
-      <c r="A82" s="42" t="s">
-        <v>26</v>
+      <c r="A82" s="52" t="s">
+        <v>45</v>
       </c>
-      <c r="B82" s="43"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="44"/>
+      <c r="B82" s="53"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="54"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -30958,9 +32821,14 @@
       <c r="T82" s="2"/>
     </row>
     <row r="83" spans="1:20" ht="12" customHeight="1">
-      <c r="A83" s="20"/>
+      <c r="A83" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="B83" s="21"/>
-      <c r="C83" s="11"/>
+      <c r="C83" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_AR_AtasDeReuni%C3%A3o.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D83" s="10"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
@@ -31067,13 +32935,15 @@
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
     </row>
-    <row r="88" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="88" spans="1:20" ht="18" customHeight="1" thickTop="1" thickBot="1">
       <c r="A88" s="16"/>
       <c r="B88" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
+      <c r="C88" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="26"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -31092,12 +32962,12 @@
       <c r="T88" s="2"/>
     </row>
     <row r="89" spans="1:20" ht="39.75" customHeight="1" thickTop="1">
-      <c r="A89" s="56" t="s">
-        <v>27</v>
+      <c r="A89" s="46" t="s">
+        <v>46</v>
       </c>
-      <c r="B89" s="57"/>
-      <c r="C89" s="57"/>
-      <c r="D89" s="58"/>
+      <c r="B89" s="47"/>
+      <c r="C89" s="47"/>
+      <c r="D89" s="48"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -31116,9 +32986,14 @@
       <c r="T89" s="2"/>
     </row>
     <row r="90" spans="1:20" ht="12" customHeight="1">
-      <c r="A90" s="20"/>
+      <c r="A90" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="B90" s="21"/>
-      <c r="C90" s="11"/>
+      <c r="C90" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/576404957d455644b03d1f04c1d601c97fe000b9/docs/Project%20Docs/MSL_CP_CronogramaDoProjeto.xlsx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D90" s="10"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
@@ -31225,13 +33100,15 @@
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
     </row>
-    <row r="95" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="95" spans="1:20" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A95" s="16"/>
       <c r="B95" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C95" s="12"/>
-      <c r="D95" s="12"/>
+      <c r="C95" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" s="26"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -31250,12 +33127,12 @@
       <c r="T95" s="2"/>
     </row>
     <row r="96" spans="1:20" ht="40.5" customHeight="1" thickTop="1">
-      <c r="A96" s="56" t="s">
-        <v>28</v>
+      <c r="A96" s="46" t="s">
+        <v>47</v>
       </c>
-      <c r="B96" s="57"/>
-      <c r="C96" s="57"/>
-      <c r="D96" s="58"/>
+      <c r="B96" s="47"/>
+      <c r="C96" s="47"/>
+      <c r="D96" s="48"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -31383,13 +33260,15 @@
       <c r="S101" s="2"/>
       <c r="T101" s="2"/>
     </row>
-    <row r="102" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="102" spans="1:20" ht="19.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A102" s="16"/>
       <c r="B102" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
+      <c r="C102" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D102" s="26"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -31408,12 +33287,12 @@
       <c r="T102" s="2"/>
     </row>
     <row r="103" spans="1:20" ht="40.5" customHeight="1" thickTop="1">
-      <c r="A103" s="56" t="s">
-        <v>29</v>
+      <c r="A103" s="46" t="s">
+        <v>48</v>
       </c>
-      <c r="B103" s="57"/>
-      <c r="C103" s="57"/>
-      <c r="D103" s="58"/>
+      <c r="B103" s="47"/>
+      <c r="C103" s="47"/>
+      <c r="D103" s="48"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
@@ -31432,9 +33311,14 @@
       <c r="T103" s="2"/>
     </row>
     <row r="104" spans="1:20" ht="12" customHeight="1">
-      <c r="A104" s="20"/>
+      <c r="A104" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="B104" s="21"/>
-      <c r="C104" s="11"/>
+      <c r="C104" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_PP_PlanoDoProjeto.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D104" s="10"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -31541,13 +33425,15 @@
       <c r="S108" s="2"/>
       <c r="T108" s="2"/>
     </row>
-    <row r="109" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="109" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A109" s="16"/>
       <c r="B109" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C109" s="12"/>
-      <c r="D109" s="12"/>
+      <c r="C109" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" s="26"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
@@ -31566,12 +33452,12 @@
       <c r="T109" s="2"/>
     </row>
     <row r="110" spans="1:20" ht="39.75" customHeight="1" thickTop="1">
-      <c r="A110" s="56" t="s">
-        <v>30</v>
+      <c r="A110" s="46" t="s">
+        <v>50</v>
       </c>
-      <c r="B110" s="57"/>
-      <c r="C110" s="57"/>
-      <c r="D110" s="58"/>
+      <c r="B110" s="47"/>
+      <c r="C110" s="47"/>
+      <c r="D110" s="48"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
@@ -31590,9 +33476,14 @@
       <c r="T110" s="2"/>
     </row>
     <row r="111" spans="1:20" ht="12" customHeight="1">
-      <c r="A111" s="20"/>
+      <c r="A111" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="B111" s="21"/>
-      <c r="C111" s="11"/>
+      <c r="C111" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/MSL_AR_AtasDeReuni%C3%A3o.docx", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D111" s="10"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -31612,9 +33503,14 @@
       <c r="T111" s="2"/>
     </row>
     <row r="112" spans="1:20" ht="12" customHeight="1">
-      <c r="A112" s="17"/>
+      <c r="A112" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="B112" s="21"/>
-      <c r="C112" s="10"/>
+      <c r="C112" s="24" t="str">
+        <f>HYPERLINK("https://github.com/nikolassupremo/PGP-2016/blob/master/docs/Project%20Docs/Termo%20de%20Compromisso%20-%20Sprint%202", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D112" s="10"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -31699,13 +33595,15 @@
       <c r="S115" s="2"/>
       <c r="T115" s="2"/>
     </row>
-    <row r="116" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="116" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A116" s="16"/>
       <c r="B116" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12"/>
+      <c r="C116" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" s="26"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
@@ -31724,12 +33622,12 @@
       <c r="T116" s="2"/>
     </row>
     <row r="117" spans="1:20" ht="39" customHeight="1" thickTop="1">
-      <c r="A117" s="56" t="s">
-        <v>31</v>
+      <c r="A117" s="46" t="s">
+        <v>51</v>
       </c>
-      <c r="B117" s="57"/>
-      <c r="C117" s="57"/>
-      <c r="D117" s="58"/>
+      <c r="B117" s="47"/>
+      <c r="C117" s="47"/>
+      <c r="D117" s="48"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
@@ -31860,10 +33758,12 @@
     <row r="123" spans="1:20" ht="12" customHeight="1" thickTop="1" thickBot="1">
       <c r="A123" s="16"/>
       <c r="B123" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C123" s="12"/>
-      <c r="D123" s="12"/>
+      <c r="C123" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D123" s="26"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
@@ -31882,12 +33782,12 @@
       <c r="T123" s="2"/>
     </row>
     <row r="124" spans="1:20" ht="54.75" customHeight="1" thickTop="1">
-      <c r="A124" s="59" t="s">
-        <v>32</v>
+      <c r="A124" s="49" t="s">
+        <v>52</v>
       </c>
-      <c r="B124" s="60"/>
-      <c r="C124" s="60"/>
-      <c r="D124" s="61"/>
+      <c r="B124" s="50"/>
+      <c r="C124" s="50"/>
+      <c r="D124" s="51"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
@@ -31906,9 +33806,14 @@
       <c r="T124" s="2"/>
     </row>
     <row r="125" spans="1:20" ht="12" customHeight="1">
-      <c r="A125" s="20"/>
+      <c r="A125" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="B125" s="21"/>
-      <c r="C125" s="11"/>
+      <c r="C125" s="24" t="str">
+        <f>HYPERLINK("https://www.dropbox.com/s/ast9g7enrjgb4jq/Sprint Retrospective - 2ª Iteração.docx?dl=0​", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D125" s="10"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
@@ -32015,13 +33920,15 @@
       <c r="S129" s="2"/>
       <c r="T129" s="2"/>
     </row>
-    <row r="130" spans="1:22" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="130" spans="1:22" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A130" s="16"/>
       <c r="B130" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C130" s="12"/>
-      <c r="D130" s="12"/>
+      <c r="C130" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D130" s="26"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
@@ -32040,12 +33947,12 @@
       <c r="T130" s="2"/>
     </row>
     <row r="131" spans="1:22" ht="90" customHeight="1" thickTop="1">
-      <c r="A131" s="42" t="s">
-        <v>33</v>
+      <c r="A131" s="52" t="s">
+        <v>53</v>
       </c>
-      <c r="B131" s="43"/>
-      <c r="C131" s="43"/>
-      <c r="D131" s="44"/>
+      <c r="B131" s="53"/>
+      <c r="C131" s="53"/>
+      <c r="D131" s="54"/>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
@@ -32064,9 +33971,14 @@
       <c r="T131" s="2"/>
     </row>
     <row r="132" spans="1:22" ht="12" customHeight="1">
-      <c r="A132" s="20"/>
+      <c r="A132" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="B132" s="21"/>
-      <c r="C132" s="11"/>
+      <c r="C132" s="24" t="str">
+        <f>HYPERLINK("https://www.dropbox.com/s/ast9g7enrjgb4jq/Sprint Retrospective - 2ª Iteração.docx?dl=0​", "X")</f>
+        <v>X</v>
+      </c>
       <c r="D132" s="10"/>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
@@ -32173,13 +34085,15 @@
       <c r="S136" s="2"/>
       <c r="T136" s="2"/>
     </row>
-    <row r="137" spans="1:22" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="137" spans="1:22" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A137" s="16"/>
       <c r="B137" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="C137" s="12"/>
-      <c r="D137" s="12"/>
+      <c r="C137" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D137" s="26"/>
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
@@ -52246,16 +54160,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="A117:D117"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A131:D131"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A103:D103"/>
     <mergeCell ref="A61:D61"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
@@ -52268,350 +54172,854 @@
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A131:D131"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A103:D103"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:D10">
-    <cfRule type="containsBlanks" dxfId="75" priority="95">
-      <formula>LEN(TRIM(A6))=0</formula>
+  <conditionalFormatting sqref="A7:D10">
+    <cfRule type="containsBlanks" dxfId="186" priority="214">
+      <formula>LEN(TRIM(A7))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B10">
-    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B6)))</formula>
+  <conditionalFormatting sqref="B7:B10">
+    <cfRule type="containsText" dxfId="185" priority="194" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B6)))</formula>
+    <cfRule type="containsText" dxfId="184" priority="193" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="183" priority="192" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D17">
-    <cfRule type="containsBlanks" dxfId="71" priority="72">
+  <conditionalFormatting sqref="A14:D17 A13:B13 D13">
+    <cfRule type="containsBlanks" dxfId="182" priority="191">
       <formula>LEN(TRIM(A13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="containsText" dxfId="70" priority="70" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="181" priority="189" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="71" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="180" priority="190" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="68" priority="69" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="179" priority="188" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:D24">
-    <cfRule type="containsBlanks" dxfId="67" priority="68">
+  <conditionalFormatting sqref="A21:D24 D20">
+    <cfRule type="containsBlanks" dxfId="178" priority="187">
       <formula>LEN(TRIM(A20))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20:B24">
-    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B20)))</formula>
+  <conditionalFormatting sqref="B21:B24">
+    <cfRule type="containsText" dxfId="177" priority="185" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B20)))</formula>
+    <cfRule type="containsText" dxfId="176" priority="186" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="175" priority="184" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27:D31">
-    <cfRule type="containsBlanks" dxfId="63" priority="64">
+  <conditionalFormatting sqref="A28:D31 D27">
+    <cfRule type="containsBlanks" dxfId="174" priority="183">
       <formula>LEN(TRIM(A27))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:B31">
-    <cfRule type="containsText" dxfId="62" priority="62" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B27)))</formula>
+  <conditionalFormatting sqref="B28:B31">
+    <cfRule type="containsText" dxfId="173" priority="181" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="63" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B27)))</formula>
+    <cfRule type="containsText" dxfId="172" priority="182" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="171" priority="180" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A34:D38">
-    <cfRule type="containsBlanks" dxfId="59" priority="60">
+  <conditionalFormatting sqref="A36:D38 A34:B35 D34:D35">
+    <cfRule type="containsBlanks" dxfId="170" priority="179">
       <formula>LEN(TRIM(A34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:B38">
-    <cfRule type="containsText" dxfId="58" priority="58" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="169" priority="177" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="59" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="168" priority="178" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="167" priority="176" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:D45">
-    <cfRule type="containsBlanks" dxfId="55" priority="56">
+  <conditionalFormatting sqref="A42:D45 D41">
+    <cfRule type="containsBlanks" dxfId="166" priority="175">
       <formula>LEN(TRIM(A41))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41:B45">
-    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B41)))</formula>
+  <conditionalFormatting sqref="B42:B45">
+    <cfRule type="containsText" dxfId="165" priority="173" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B41)))</formula>
+    <cfRule type="containsText" dxfId="164" priority="174" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="163" priority="172" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48:D52">
-    <cfRule type="containsBlanks" dxfId="51" priority="52">
+  <conditionalFormatting sqref="A49:D52 A48:B48 D48">
+    <cfRule type="containsBlanks" dxfId="162" priority="171">
       <formula>LEN(TRIM(A48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:B52">
-    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="161" priority="169" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="51" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="160" priority="170" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="159" priority="168" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A55:D59">
-    <cfRule type="containsBlanks" dxfId="47" priority="48">
+  <conditionalFormatting sqref="A56:D59 A55:B55 D55">
+    <cfRule type="containsBlanks" dxfId="158" priority="167">
       <formula>LEN(TRIM(A55))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55:B59">
-    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="157" priority="165" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="47" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="156" priority="166" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="155" priority="164" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A62:D66">
-    <cfRule type="containsBlanks" dxfId="43" priority="44">
+  <conditionalFormatting sqref="A63:D66 A62:B62 D62">
+    <cfRule type="containsBlanks" dxfId="154" priority="163">
       <formula>LEN(TRIM(A62))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:B66">
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="153" priority="161" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="152" priority="162" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="151" priority="160" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69:D73">
-    <cfRule type="containsBlanks" dxfId="39" priority="40">
+  <conditionalFormatting sqref="A70:D73 D69">
+    <cfRule type="containsBlanks" dxfId="150" priority="159">
       <formula>LEN(TRIM(A69))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69:B73">
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B69)))</formula>
+  <conditionalFormatting sqref="B70:B73">
+    <cfRule type="containsText" dxfId="149" priority="157" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B69)))</formula>
+    <cfRule type="containsText" dxfId="148" priority="158" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="147" priority="156" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A76:D80">
-    <cfRule type="containsBlanks" dxfId="35" priority="36">
+    <cfRule type="containsBlanks" dxfId="146" priority="155">
       <formula>LEN(TRIM(A76))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:B80">
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="145" priority="153" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="144" priority="154" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="143" priority="152" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B77)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A83:D87">
-    <cfRule type="containsBlanks" dxfId="31" priority="32">
+  <conditionalFormatting sqref="A84:D87 D83">
+    <cfRule type="containsBlanks" dxfId="142" priority="151">
       <formula>LEN(TRIM(A83))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B83:B87">
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B83)))</formula>
+  <conditionalFormatting sqref="B84:B87">
+    <cfRule type="containsText" dxfId="141" priority="149" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B84)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B83)))</formula>
+    <cfRule type="containsText" dxfId="140" priority="150" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="139" priority="148" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B84)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A90:D94">
-    <cfRule type="containsBlanks" dxfId="27" priority="28">
+  <conditionalFormatting sqref="A91:D94 D90">
+    <cfRule type="containsBlanks" dxfId="138" priority="147">
       <formula>LEN(TRIM(A90))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:B94">
-    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B90)))</formula>
+  <conditionalFormatting sqref="B91:B94">
+    <cfRule type="containsText" dxfId="137" priority="145" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B90)))</formula>
+    <cfRule type="containsText" dxfId="136" priority="146" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="135" priority="144" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97:D101">
-    <cfRule type="containsBlanks" dxfId="23" priority="24">
+    <cfRule type="containsBlanks" dxfId="134" priority="143">
       <formula>LEN(TRIM(A97))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97:B101">
-    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="133" priority="141" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="132" priority="142" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="131" priority="140" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B98)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A104:D108">
-    <cfRule type="containsBlanks" dxfId="19" priority="20">
+  <conditionalFormatting sqref="A105:D108 D104">
+    <cfRule type="containsBlanks" dxfId="130" priority="139">
       <formula>LEN(TRIM(A104))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B104:B108">
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B104)))</formula>
+  <conditionalFormatting sqref="B105:B108">
+    <cfRule type="containsText" dxfId="129" priority="137" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B104)))</formula>
+    <cfRule type="containsText" dxfId="128" priority="138" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="127" priority="136" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B105)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A111:D115">
-    <cfRule type="containsBlanks" dxfId="15" priority="16">
+  <conditionalFormatting sqref="A113:D115 D111:D112">
+    <cfRule type="containsBlanks" dxfId="126" priority="135">
       <formula>LEN(TRIM(A111))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B111:B115">
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B111)))</formula>
+  <conditionalFormatting sqref="B113:B115">
+    <cfRule type="containsText" dxfId="125" priority="133" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B111)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B112">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",B112)))</formula>
+    <cfRule type="containsText" dxfId="124" priority="134" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A118:D122">
-    <cfRule type="containsBlanks" dxfId="11" priority="12">
+    <cfRule type="containsBlanks" dxfId="123" priority="131">
       <formula>LEN(TRIM(A118))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B118:B122">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="AP">
+    <cfRule type="containsText" dxfId="122" priority="129" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B118)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="121" priority="130" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B118)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B119">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="120" priority="128" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B119)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A125:D129">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+  <conditionalFormatting sqref="A126:D129 D125">
+    <cfRule type="containsBlanks" dxfId="119" priority="127">
       <formula>LEN(TRIM(A125))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B125:B129">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="AP">
+  <conditionalFormatting sqref="B126:B129">
+    <cfRule type="containsText" dxfId="118" priority="125" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B126)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="126" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B126)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B126">
+    <cfRule type="containsText" dxfId="116" priority="124" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",B126)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A133:D136 D132">
+    <cfRule type="containsBlanks" dxfId="115" priority="123">
+      <formula>LEN(TRIM(A132))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B133:B136">
+    <cfRule type="containsText" dxfId="114" priority="121" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B133)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="113" priority="122" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B133)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B133">
+    <cfRule type="containsText" dxfId="112" priority="120" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",B133)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:D6">
+    <cfRule type="containsBlanks" dxfId="111" priority="119">
+      <formula>LEN(TRIM(A6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="containsText" dxfId="110" priority="117" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="118" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="containsText" dxfId="108" priority="116" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="containsBlanks" dxfId="107" priority="115">
+      <formula>LEN(TRIM(C13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:C20">
+    <cfRule type="containsBlanks" dxfId="106" priority="114">
+      <formula>LEN(TRIM(A20))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="containsText" dxfId="105" priority="112" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="104" priority="113" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="containsText" dxfId="103" priority="111" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",B20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:B27">
+    <cfRule type="containsBlanks" dxfId="102" priority="110">
+      <formula>LEN(TRIM(A27))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="containsText" dxfId="101" priority="108" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="109" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="containsBlanks" dxfId="99" priority="107">
+      <formula>LEN(TRIM(C27))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsBlanks" dxfId="98" priority="106">
+      <formula>LEN(TRIM(C34))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsBlanks" dxfId="97" priority="105">
+      <formula>LEN(TRIM(C35))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:C41">
+    <cfRule type="containsBlanks" dxfId="96" priority="104">
+      <formula>LEN(TRIM(A41))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="containsText" dxfId="95" priority="102" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="103" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="containsText" dxfId="93" priority="101" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",B41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsBlanks" dxfId="92" priority="97">
+      <formula>LEN(TRIM(C48))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="containsBlanks" dxfId="91" priority="96">
+      <formula>LEN(TRIM(C55))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="containsBlanks" dxfId="90" priority="95">
+      <formula>LEN(TRIM(C62))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90:B90">
+    <cfRule type="containsBlanks" dxfId="89" priority="94">
+      <formula>LEN(TRIM(A90))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B90">
+    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B90)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="87" priority="93" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B90">
+    <cfRule type="containsText" dxfId="86" priority="91" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",B90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C90">
+    <cfRule type="containsBlanks" dxfId="85" priority="90">
+      <formula>LEN(TRIM(C90))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104:B104">
+    <cfRule type="containsBlanks" dxfId="84" priority="89">
+      <formula>LEN(TRIM(A104))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B104">
+    <cfRule type="containsText" dxfId="83" priority="87" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B104)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="88" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B104)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C104">
+    <cfRule type="containsBlanks" dxfId="81" priority="86">
+      <formula>LEN(TRIM(C104))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A132:B132">
+    <cfRule type="containsBlanks" dxfId="80" priority="85">
+      <formula>LEN(TRIM(A132))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B132">
+    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B132)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B132)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C132">
+    <cfRule type="containsBlanks" dxfId="77" priority="82">
+      <formula>LEN(TRIM(C132))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A125:B125">
+    <cfRule type="containsBlanks" dxfId="76" priority="81">
+      <formula>LEN(TRIM(A125))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
+    <cfRule type="containsText" dxfId="75" priority="79" operator="containsText" text="AP">
       <formula>NOT(ISERROR(SEARCH("AP",B125)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="74" priority="80" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",B125)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B126">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",B126)))</formula>
+  <conditionalFormatting sqref="C125">
+    <cfRule type="containsBlanks" dxfId="73" priority="78">
+      <formula>LEN(TRIM(C125))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A132:D136">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A132))=0</formula>
+  <conditionalFormatting sqref="A111:B111">
+    <cfRule type="containsBlanks" dxfId="72" priority="77">
+      <formula>LEN(TRIM(A111))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B132:B136">
+  <conditionalFormatting sqref="B111">
+    <cfRule type="containsText" dxfId="71" priority="75" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B111)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="76" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B111)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C111">
+    <cfRule type="containsBlanks" dxfId="69" priority="74">
+      <formula>LEN(TRIM(C111))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83:B83">
+    <cfRule type="containsBlanks" dxfId="68" priority="73">
+      <formula>LEN(TRIM(A83))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83">
+    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B83)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C83">
+    <cfRule type="containsBlanks" dxfId="65" priority="70">
+      <formula>LEN(TRIM(C83))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A112:B112">
+    <cfRule type="containsBlanks" dxfId="64" priority="69">
+      <formula>LEN(TRIM(A112))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B112">
+    <cfRule type="containsText" dxfId="63" priority="67" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B112)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="68" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B112)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C112">
+    <cfRule type="containsBlanks" dxfId="61" priority="66">
+      <formula>LEN(TRIM(C112))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69:C69">
+    <cfRule type="containsBlanks" dxfId="60" priority="65">
+      <formula>LEN(TRIM(A69))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
+    <cfRule type="containsText" dxfId="59" priority="63" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",B69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="64" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",B69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
+    <cfRule type="containsText" dxfId="57" priority="62" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",B69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="containsText" dxfId="56" priority="59" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="60" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:D11">
+    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="containsText" dxfId="53" priority="53" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="54" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:D18">
+    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="51" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:D25">
+    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="containsText" dxfId="47" priority="47" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="48" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:D32">
+    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:D39">
+    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46:D46">
+    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53:D53">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C60)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:D60">
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67:D67">
+    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C74)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C74)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74:D74">
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C74)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C81">
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C81)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C81:D81">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C81)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C88)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88:D88">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C95">
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C95)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C95)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C95:D95">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C95)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C102">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C102)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C102)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C102:D102">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C102)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C109">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C109)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C109)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C109:D109">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C109)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C116">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C116)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C116)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C116:D116">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C116)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C130">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C130)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C130)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C130:D130">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C130)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C137">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="AP">
+      <formula>NOT(ISERROR(SEARCH("AP",C137)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH("A",C137)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C137:D137">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",C137)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C123">
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="AP">
-      <formula>NOT(ISERROR(SEARCH("AP",B132)))</formula>
+      <formula>NOT(ISERROR(SEARCH("AP",C123)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH("A",B132)))</formula>
+      <formula>NOT(ISERROR(SEARCH("A",C123)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B133">
+  <conditionalFormatting sqref="C123:D123">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",B133)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NA",C123)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>